<commit_message>
[CHANGED]: schema.js since I feel like the format is actually the format to be imported to odoo
</commit_message>
<xml_diff>
--- a/tests/spreadsheets/sample_draft_quote.xlsx
+++ b/tests/spreadsheets/sample_draft_quote.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Web\React-Web\odoo_quote_import\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Web\React-Web\odoo_quote_import\tests\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{774D9F1C-3A28-4386-82ED-4E071E56D3B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE6F54EB-CFC0-4796-8BD9-49929CDEDEAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3975" yWindow="1665" windowWidth="21600" windowHeight="11295" xr2:uid="{02BBA245-1A48-407B-B43F-BD3301737075}"/>
+    <workbookView xWindow="3285" yWindow="1890" windowWidth="21600" windowHeight="11295" xr2:uid="{02BBA245-1A48-407B-B43F-BD3301737075}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,13 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
-  <si>
-    <t>Display Type</t>
-  </si>
-  <si>
-    <t>Product</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Description</t>
   </si>
@@ -67,24 +61,19 @@
   </si>
   <si>
     <t>Setup Server 2</t>
+  </si>
+  <si>
+    <t>Display</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -141,29 +130,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -513,101 +501,95 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCCB795F-36DD-473D-9E0C-9AD0A002F0A1}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="B3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
     </row>
-    <row r="2" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="8">
+        <v>2</v>
+      </c>
+      <c r="D4" s="8">
+        <v>1600</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-    </row>
-    <row r="4" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="9">
-        <v>2</v>
-      </c>
-      <c r="E4" s="9">
-        <v>1600</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B5" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A2 A4:A5">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="1">
+      <formula>LEN(TRIM(A2))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B2:B5">
-    <cfRule type="notContainsBlanks" dxfId="3" priority="1">
-      <formula>LEN(TRIM(B2))&gt;0</formula>
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>NOT(ISBLANK(A2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C5">
-    <cfRule type="expression" dxfId="2" priority="2">
-      <formula>NOT(ISBLANK(B2))</formula>
+    <cfRule type="expression" dxfId="1" priority="3">
+      <formula>NOT(ISBLANK(A2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D5">
-    <cfRule type="expression" dxfId="1" priority="3">
-      <formula>NOT(ISBLANK(B2))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E5">
     <cfRule type="expression" dxfId="0" priority="4">
-      <formula>NOT(ISBLANK(B2))</formula>
+      <formula>NOT(ISBLANK(A2))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>